<commit_message>
updated templates, added instructions, changed some layout formatting
</commit_message>
<xml_diff>
--- a/public/data/RippleTemplate_Basic.xlsx
+++ b/public/data/RippleTemplate_Basic.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\adalecki\projects\react\stjudehtb\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\adalecki\Projects\react\ripple\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87EBE402-16B6-47E2-9DE9-1210DF629326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0D9A5D-3BEA-4FD2-BB67-720D0D843296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{78FBB280-6DFE-437C-B3D1-3C5CE54962AD}"/>
+    <workbookView xWindow="36495" yWindow="-10140" windowWidth="28800" windowHeight="15345" xr2:uid="{78FBB280-6DFE-437C-B3D1-3C5CE54962AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Patterns" sheetId="3" r:id="rId1"/>
     <sheet name="Layout" sheetId="1" r:id="rId2"/>
     <sheet name="Compounds" sheetId="2" r:id="rId3"/>
     <sheet name="Barcodes" sheetId="4" r:id="rId4"/>
+    <sheet name="Assay" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="233">
   <si>
     <t>Replicates</t>
   </si>
@@ -711,6 +712,33 @@
   </si>
   <si>
     <t>Volume (µL)</t>
+  </si>
+  <si>
+    <t>Setting</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>DMSO Tolerance</t>
+  </si>
+  <si>
+    <t>Well Volume (µL)</t>
+  </si>
+  <si>
+    <t>Backfill (µL)</t>
+  </si>
+  <si>
+    <t>Allowed Error</t>
+  </si>
+  <si>
+    <t>Destination Replicates</t>
+  </si>
+  <si>
+    <t>Use Intermediate Plates</t>
+  </si>
+  <si>
+    <t>DMSO Normalization</t>
   </si>
 </sst>
 </file>
@@ -1072,7 +1100,7 @@
   <dimension ref="A1:AH32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2927,4 +2955,83 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{155CF110-73CB-449A-8D25-F53C9CBD73AC}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="A1:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>